<commit_message>
add sections + picture to report
</commit_message>
<xml_diff>
--- a/Assignment3 - Phase2/Book1.xlsx
+++ b/Assignment3 - Phase2/Book1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="12">
   <si>
     <t>A9-A9-A9</t>
   </si>
@@ -53,10 +53,13 @@
     <t>dividing line between 2 thread</t>
   </si>
   <si>
-    <t>2/3 on main, 1/3 on thread</t>
+    <t xml:space="preserve">by putting 13 in the </t>
   </si>
   <si>
-    <t xml:space="preserve">by putting 13 in the </t>
+    <t xml:space="preserve">13 on the first, </t>
+  </si>
+  <si>
+    <t>2/3 on the first core, 1/3 on the second</t>
   </si>
 </sst>
 </file>
@@ -262,13 +265,13 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$E$6:$E$8</c:f>
+              <c:f>Sheet1!$E$6:$E$9</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>A9-A9-A9</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>A15-A9</c:v>
                 </c:pt>
               </c:strCache>
@@ -276,14 +279,20 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$6:$F$8</c:f>
+              <c:f>Sheet1!$F$6:$F$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>46900802000</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="0%">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>32272300000</c:v>
                 </c:pt>
               </c:numCache>
@@ -379,13 +388,13 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$E$6:$E$8</c:f>
+              <c:f>Sheet1!$E$6:$E$9</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>A9-A9-A9</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>A15-A9</c:v>
                 </c:pt>
               </c:strCache>
@@ -393,17 +402,20 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$6:$G$8</c:f>
+              <c:f>Sheet1!$G$6:$G$9</c:f>
               <c:numCache>
-                <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0" formatCode="General">
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
                   <c:v>47172909000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.01661765662813</c:v>
-                </c:pt>
-                <c:pt idx="2" formatCode="General">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="0%">
+                  <c:v>-1.6617656628129973E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>32808590000</c:v>
                 </c:pt>
               </c:numCache>
@@ -499,13 +511,13 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$E$6:$E$8</c:f>
+              <c:f>Sheet1!$E$6:$E$9</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>A9-A9-A9</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>A15-A9</c:v>
                 </c:pt>
               </c:strCache>
@@ -513,17 +525,20 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$6:$H$8</c:f>
+              <c:f>Sheet1!$H$6:$H$9</c:f>
               <c:numCache>
-                <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0" formatCode="General">
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
                   <c:v>27626245000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.82426579450488502</c:v>
-                </c:pt>
-                <c:pt idx="2" formatCode="General">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="0%">
+                  <c:v>0.17573420549511498</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>26600953000</c:v>
                 </c:pt>
               </c:numCache>
@@ -544,7 +559,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2/3 on main, 1/3 on thread</c:v>
+                  <c:v>13 on the first, </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -619,13 +634,13 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$E$6:$E$8</c:f>
+              <c:f>Sheet1!$E$6:$E$9</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>A9-A9-A9</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>A15-A9</c:v>
                 </c:pt>
               </c:strCache>
@@ -633,17 +648,20 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$I$6:$I$8</c:f>
+              <c:f>Sheet1!$I$6:$I$9</c:f>
               <c:numCache>
-                <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0" formatCode="General">
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
                   <c:v>19577778000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.76970987503214827</c:v>
-                </c:pt>
-                <c:pt idx="2" formatCode="General">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="0%">
+                  <c:v>0.23029012496785173</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>24840308000</c:v>
                 </c:pt>
               </c:numCache>
@@ -866,6 +884,40 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Performance increase in percentage A9-A9-A9</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>(higher is better)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -899,20 +951,12 @@
     <c:plotArea>
       <c:layout/>
       <c:barChart>
-        <c:barDir val="bar"/>
+        <c:barDir val="col"/>
         <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$E$5</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
           <c:spPr>
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -938,7 +982,7 @@
                   <c:v>dividing line between 2 thread</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2/3 on main, 1/3 on thread</c:v>
+                  <c:v>13 on the first, </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -949,228 +993,24 @@
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0058017557993997</c:v>
+                  <c:v>-5.8017557993996771E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.58903566297224508</c:v>
+                  <c:v>0.41096433702775492</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.41742949299672955</c:v>
+                  <c:v>0.58257050700327051</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-B89C-4C5A-B94B-8F7C7353D3B0}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$E$6</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>A9-A9-A9</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$F$4:$I$4</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>default</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>one line of the picture  is placed on thread</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>dividing line between 2 thread</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2/3 on main, 1/3 on thread</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$F$6:$I$6</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>46900802000</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>47172909000</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>27626245000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>19577778000</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-B89C-4C5A-B94B-8F7C7353D3B0}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$E$7</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$F$4:$I$4</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>default</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>one line of the picture  is placed on thread</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>dividing line between 2 thread</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2/3 on main, 1/3 on thread</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$F$7:$I$7</c:f>
-              <c:numCache>
-                <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="1">
-                  <c:v>1.01661765662813</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.82426579450488502</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.76970987503214827</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-B89C-4C5A-B94B-8F7C7353D3B0}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$E$8</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>A15-A9</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent4"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$F$4:$I$4</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>default</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>one line of the picture  is placed on thread</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>dividing line between 2 thread</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2/3 on main, 1/3 on thread</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$F$8:$I$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>32272300000</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>32808590000</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>26600953000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>24840308000</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-B89C-4C5A-B94B-8F7C7353D3B0}"/>
+              <c16:uniqueId val="{00000000-D432-43C5-99AC-E90D8E1E8F11}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1182,17 +1022,18 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="182"/>
-        <c:axId val="333115568"/>
-        <c:axId val="333115896"/>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="480619008"/>
+        <c:axId val="480617040"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="333115568"/>
+        <c:axId val="480619008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="l"/>
+        <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1230,7 +1071,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="333115896"/>
+        <c:crossAx val="480617040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1238,12 +1079,13 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="333115896"/>
+        <c:axId val="480617040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="-1.0000000000000002E-2"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="b"/>
+        <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -1258,7 +1100,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1289,7 +1131,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="333115568"/>
+        <c:crossAx val="480619008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1301,8 +1143,110 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Performance increase in percentage A15-A9</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1400">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>(higher is better)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1400">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.17096361607011573"/>
+          <c:y val="2.7117225416740508E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1316,7 +1260,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -1331,7 +1275,203 @@
           <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
-    </c:legend>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$F$7:$I$7</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>default</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>one line of the picture  is placed on thread</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>dividing line between 2 thread</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2/3 on the first core, 1/3 on the second</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$8:$I$8</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-1.6617656628129973E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.17573420549511498</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.23029012496785173</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9223-4018-8A1D-93C96AF59805}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="475849448"/>
+        <c:axId val="475847152"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="475849448"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="b" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="475847152"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="475847152"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="-2.0000000000000004E-2"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="475849448"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -1449,6 +1589,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
   <cs:axisTitle>
@@ -1955,7 +2135,7 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -2159,23 +2339,22 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -2280,8 +2459,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2413,20 +2592,522 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
         <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -2465,13 +3146,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>82550</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2499,23 +3180,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>227135</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>123093</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>170962</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>54708</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>80597</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>82062</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>200270</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>166077</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
+        <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{650C97C5-38DD-4861-AD0C-FC70B9992A9B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{007FF256-D3F8-4285-AC8A-A835238FC57F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2528,6 +3209,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>393210</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>34956</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1196731</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>157581</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ED023932-2F4C-4C3E-930E-AB1455E364A6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2833,10 +3550,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D9" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView tabSelected="1" topLeftCell="F16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2920,24 +3637,28 @@
         <v>8</v>
       </c>
       <c r="I4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J4" t="s">
         <v>9</v>
-      </c>
-      <c r="J4" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="F5" s="3">
+        <f>1-F6/F6</f>
+        <v>0</v>
+      </c>
       <c r="G5" s="2">
-        <f>G6/F6</f>
-        <v>1.0058017557993997</v>
+        <f>1-G6/F6</f>
+        <v>-5.8017557993996771E-3</v>
       </c>
       <c r="H5" s="2">
-        <f>H6/F6</f>
-        <v>0.58903566297224508</v>
+        <f>1-H6/F6</f>
+        <v>0.41096433702775492</v>
       </c>
       <c r="I5" s="2">
-        <f>I6/F6</f>
-        <v>0.41742949299672955</v>
+        <f>1-I6/F6</f>
+        <v>0.58257050700327051</v>
       </c>
       <c r="J5" s="2">
         <f>J6/F6</f>
@@ -2967,37 +3688,55 @@
         <v>19577778000</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="G7" s="3">
-        <f>G8/F8</f>
-        <v>1.01661765662813</v>
-      </c>
-      <c r="H7" s="3">
-        <f>H8/F8</f>
-        <v>0.82426579450488502</v>
-      </c>
-      <c r="I7" s="3">
-        <f>I8/F8</f>
-        <v>0.76970987503214827</v>
+    <row r="7" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="F7" t="s">
+        <v>2</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+      <c r="F8" s="3">
+        <f>1-F9/F9</f>
+        <v>0</v>
+      </c>
+      <c r="G8" s="3">
+        <f>1-G9/F9</f>
+        <v>-1.6617656628129973E-2</v>
+      </c>
+      <c r="H8" s="3">
+        <f>1-H9/F9</f>
+        <v>0.17573420549511498</v>
+      </c>
+      <c r="I8" s="3">
+        <f>1-I9/F9</f>
+        <v>0.23029012496785173</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>1</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E9" t="s">
         <v>1</v>
       </c>
-      <c r="F8">
+      <c r="F9">
         <v>32272300000</v>
       </c>
-      <c r="G8">
+      <c r="G9">
         <v>32808590000</v>
       </c>
-      <c r="H8">
+      <c r="H9">
         <v>26600953000</v>
       </c>
-      <c r="I8">
+      <c r="I9">
         <v>24840308000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
abstract, finished pixels line on thread, add new pictures, conclusion
</commit_message>
<xml_diff>
--- a/Assignment3 - Phase2/Book1.xlsx
+++ b/Assignment3 - Phase2/Book1.xlsx
@@ -56,10 +56,10 @@
     <t xml:space="preserve">by putting 13 in the </t>
   </si>
   <si>
-    <t xml:space="preserve">13 on the first, </t>
+    <t>2/3 on the first core, 1/3 on the second</t>
   </si>
   <si>
-    <t>2/3 on the first core, 1/3 on the second</t>
+    <t>13 on the first, 6 on the second and 11 on the third thread</t>
   </si>
 </sst>
 </file>
@@ -265,13 +265,13 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$E$6:$E$9</c:f>
+              <c:f>Sheet1!$E$5:$E$7</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>A9-A9-A9</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="2">
                   <c:v>A15-A9</c:v>
                 </c:pt>
               </c:strCache>
@@ -279,20 +279,17 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$6:$F$9</c:f>
+              <c:f>Sheet1!$F$5:$F$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>46900802000</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="2" formatCode="0%">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="2">
                   <c:v>32272300000</c:v>
                 </c:pt>
               </c:numCache>
@@ -388,13 +385,13 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$E$6:$E$9</c:f>
+              <c:f>Sheet1!$E$5:$E$7</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>A9-A9-A9</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="2">
                   <c:v>A15-A9</c:v>
                 </c:pt>
               </c:strCache>
@@ -402,20 +399,17 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$6:$G$9</c:f>
+              <c:f>Sheet1!$G$5:$G$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>47172909000</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="2" formatCode="0%">
-                  <c:v>-1.6617656628129973E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="2">
                   <c:v>32808590000</c:v>
                 </c:pt>
               </c:numCache>
@@ -511,13 +505,13 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$E$6:$E$9</c:f>
+              <c:f>Sheet1!$E$5:$E$7</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>A9-A9-A9</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="2">
                   <c:v>A15-A9</c:v>
                 </c:pt>
               </c:strCache>
@@ -525,20 +519,17 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$6:$H$9</c:f>
+              <c:f>Sheet1!$H$5:$H$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>27626245000</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="2" formatCode="0%">
-                  <c:v>0.17573420549511498</c:v>
-                </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="2">
                   <c:v>26600953000</c:v>
                 </c:pt>
               </c:numCache>
@@ -559,7 +550,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>13 on the first, </c:v>
+                  <c:v>13 on the first, 6 on the second and 11 on the third thread</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -634,13 +625,13 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$E$6:$E$9</c:f>
+              <c:f>Sheet1!$E$5:$E$7</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>A9-A9-A9</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="2">
                   <c:v>A15-A9</c:v>
                 </c:pt>
               </c:strCache>
@@ -648,20 +639,17 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$I$6:$I$9</c:f>
+              <c:f>Sheet1!$I$5:$I$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>19577778000</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="2" formatCode="0%">
-                  <c:v>0.23029012496785173</c:v>
-                </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="2">
                   <c:v>24840308000</c:v>
                 </c:pt>
               </c:numCache>
@@ -904,16 +892,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Performance increase in percentage A9-A9-A9</a:t>
-            </a:r>
-          </a:p>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>(higher is better)</a:t>
+              <a:t>Performance in tick of A9-A9-A9</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -982,7 +961,7 @@
                   <c:v>dividing line between 2 thread</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>13 on the first, </c:v>
+                  <c:v>13 on the first, 6 on the second and 11 on the third thread</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -991,19 +970,19 @@
             <c:numRef>
               <c:f>Sheet1!$F$5:$I$5</c:f>
               <c:numCache>
-                <c:formatCode>0%</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>46900802000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-5.8017557993996771E-3</c:v>
+                  <c:v>47172909000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.41096433702775492</c:v>
+                  <c:v>27626245000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.58257050700327051</c:v>
+                  <c:v>19577778000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1100,7 +1079,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1217,21 +1196,7 @@
               <a:rPr lang="en-US" sz="1400" b="0" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
-              <a:t>Performance increase in percentage A15-A9</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US" sz="1400">
-              <a:effectLst/>
-            </a:endParaRPr>
-          </a:p>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US" sz="1400" b="0" i="0" baseline="0">
-                <a:effectLst/>
-              </a:rPr>
-              <a:t>(higher is better)</a:t>
+              <a:t>Performance in tick of A15-A9</a:t>
             </a:r>
             <a:endParaRPr lang="en-US" sz="1400">
               <a:effectLst/>
@@ -1298,7 +1263,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$F$7:$I$7</c:f>
+              <c:f>Sheet1!$F$6:$I$6</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -1318,21 +1283,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$8:$I$8</c:f>
+              <c:f>Sheet1!$F$7:$I$7</c:f>
               <c:numCache>
-                <c:formatCode>0%</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>32272300000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-1.6617656628129973E-2</c:v>
+                  <c:v>32808590000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.17573420549511498</c:v>
+                  <c:v>26600953000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.23029012496785173</c:v>
+                  <c:v>24840308000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1429,7 +1394,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3146,13 +3111,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>82550</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3181,15 +3146,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>170962</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:colOff>60740</xdr:colOff>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>54708</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>200270</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>166077</xdr:rowOff>
+      <xdr:colOff>200271</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>33131</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3218,13 +3183,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>393210</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>34956</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>1196731</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:colOff>1325217</xdr:colOff>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>157581</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3550,10 +3515,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J35" sqref="J35"/>
+    <sheetView tabSelected="1" topLeftCell="E14" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3636,108 +3601,104 @@
       <c r="H4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I4" t="s">
-        <v>10</v>
+      <c r="I4" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="J4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="F5" s="3">
-        <f>1-F6/F6</f>
+      <c r="A5" t="s">
         <v>0</v>
       </c>
-      <c r="G5" s="2">
-        <f>1-G6/F6</f>
-        <v>-5.8017557993996771E-3</v>
-      </c>
-      <c r="H5" s="2">
-        <f>1-H6/F6</f>
-        <v>0.41096433702775492</v>
-      </c>
-      <c r="I5" s="2">
-        <f>1-I6/F6</f>
-        <v>0.58257050700327051</v>
-      </c>
-      <c r="J5" s="2">
-        <f>J6/F6</f>
-        <v>0.41742949299672955</v>
+      <c r="E5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>46900802000</v>
+      </c>
+      <c r="G5">
+        <v>47172909000</v>
+      </c>
+      <c r="H5">
+        <v>27626245000</v>
+      </c>
+      <c r="I5">
+        <v>19577778000</v>
+      </c>
+      <c r="J5">
+        <v>19577778000</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>0</v>
-      </c>
-      <c r="E6" t="s">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>46900802000</v>
-      </c>
-      <c r="G6">
-        <v>47172909000</v>
-      </c>
-      <c r="H6">
-        <v>27626245000</v>
-      </c>
-      <c r="I6">
-        <v>19577778000</v>
-      </c>
-      <c r="J6">
-        <v>19577778000</v>
+    <row r="6" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="F6" t="s">
+        <v>2</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="F7" t="s">
-        <v>2</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>11</v>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>32272300000</v>
+      </c>
+      <c r="G7">
+        <v>32808590000</v>
+      </c>
+      <c r="H7">
+        <v>26600953000</v>
+      </c>
+      <c r="I7">
+        <v>24840308000</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="F8" s="3">
-        <f>1-F9/F9</f>
+        <f>1-F7/F7</f>
         <v>0</v>
       </c>
       <c r="G8" s="3">
-        <f>1-G9/F9</f>
+        <f>1-G7/F7</f>
         <v>-1.6617656628129973E-2</v>
       </c>
       <c r="H8" s="3">
-        <f>1-H9/F9</f>
+        <f>1-H7/F7</f>
         <v>0.17573420549511498</v>
       </c>
       <c r="I8" s="3">
-        <f>1-I9/F9</f>
+        <f>1-I7/F7</f>
         <v>0.23029012496785173</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>1</v>
-      </c>
-      <c r="E9" t="s">
-        <v>1</v>
-      </c>
-      <c r="F9">
-        <v>32272300000</v>
-      </c>
-      <c r="G9">
-        <v>32808590000</v>
-      </c>
-      <c r="H9">
-        <v>26600953000</v>
-      </c>
-      <c r="I9">
-        <v>24840308000</v>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="F10" s="3">
+        <f>1-F5/F5</f>
+        <v>0</v>
+      </c>
+      <c r="G10" s="2">
+        <f>1-G5/F5</f>
+        <v>-5.8017557993996771E-3</v>
+      </c>
+      <c r="H10" s="2">
+        <f>1-H5/F5</f>
+        <v>0.41096433702775492</v>
+      </c>
+      <c r="I10" s="2">
+        <f>1-I5/F5</f>
+        <v>0.58257050700327051</v>
       </c>
     </row>
   </sheetData>

</xml_diff>